<commit_message>
first three years data filled
</commit_message>
<xml_diff>
--- a/result/FinalResult.xlsx
+++ b/result/FinalResult.xlsx
@@ -1,19 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MalwareParser\result\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Spring 2018\MalwareParser\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF53E070-BB61-42F3-9842-F3956D5DD9AA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31DC541F-A255-45ED-B8DD-D4F4DEF13534}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808" xr2:uid="{CBE23980-1FF3-45A1-8BB9-29F4BBABBC95}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8805" activeTab="3" xr2:uid="{CBE23980-1FF3-45A1-8BB9-29F4BBABBC95}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="2018" sheetId="2" r:id="rId1"/>
+    <sheet name="2017" sheetId="1" r:id="rId2"/>
+    <sheet name="2016" sheetId="3" r:id="rId3"/>
+    <sheet name="2015" sheetId="4" r:id="rId4"/>
+    <sheet name="2014" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="43">
   <si>
     <t>oracle</t>
   </si>
@@ -148,6 +152,12 @@
   </si>
   <si>
     <t>Keyword</t>
+  </si>
+  <si>
+    <t>android</t>
+  </si>
+  <si>
+    <t>Frequency</t>
   </si>
 </sst>
 </file>
@@ -498,235 +508,1526 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CCA1CF2-BE1B-4C34-8AD2-DE4EAEE537EC}">
+  <dimension ref="A1:B42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFA8A365-071E-4679-86A5-A7CE8FDCB91A}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:B42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2">
+        <v>2449</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>2941</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>4233</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>3314</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>2520</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>2605</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>1219</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>1233</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42">
+        <v>654</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EFD2CA7-7F30-488B-8E54-5F2CA70D697E}">
+  <dimension ref="A1:B42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>4745</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>1805</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>2368</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42">
+        <v>532</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7402A537-7229-458F-959E-9C69C3F89CF9}">
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.68359375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>40</v>
       </c>
-      <c r="B1">
-        <v>2018</v>
-      </c>
-      <c r="C1">
-        <v>2017</v>
-      </c>
-      <c r="D1">
-        <v>2016</v>
-      </c>
-      <c r="E1">
-        <v>2015</v>
-      </c>
-      <c r="F1">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55B06241-76DE-4C39-BAB8-64152090AE5B}">
+  <dimension ref="A1:B42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>